<commit_message>
[Sequece Diagram] finish Sequence Diagram
</commit_message>
<xml_diff>
--- a/O2/UML/Sequence_diagram/SequenceDiagram.xlsx
+++ b/O2/UML/Sequence_diagram/SequenceDiagram.xlsx
@@ -8,16 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\OOAD\O2\UML\Sequence_diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA892AEE-3255-4929-9387-38973960A7C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2F25C278-CBAF-4715-92E5-2733966C93C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" firstSheet="2" activeTab="4" xr2:uid="{D5312A71-8C59-459C-9C61-B9E693DC5B91}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" firstSheet="10" activeTab="10" xr2:uid="{D5312A71-8C59-459C-9C61-B9E693DC5B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Đăng nhập" sheetId="1" r:id="rId1"/>
     <sheet name="Tạo hồ sơ bệnh nhân" sheetId="2" r:id="rId2"/>
     <sheet name="Tạo hồ sơ bệnh án" sheetId="3" r:id="rId3"/>
-    <sheet name="Báo cáo" sheetId="4" r:id="rId4"/>
-    <sheet name="Lấy danh sách bệnh nhân chờ" sheetId="5" r:id="rId5"/>
+    <sheet name="Thanh toán" sheetId="8" r:id="rId4"/>
+    <sheet name="Báo cáo" sheetId="4" r:id="rId5"/>
+    <sheet name="Lấy danh sách bệnh nhân chờ" sheetId="5" r:id="rId6"/>
+    <sheet name="Ghi thông tin khám bệnh" sheetId="6" r:id="rId7"/>
+    <sheet name="Tạo danh sách xét nghiệm" sheetId="7" r:id="rId8"/>
+    <sheet name="Lấy lết quả xét nghiệm" sheetId="9" r:id="rId9"/>
+    <sheet name="Kê đơn thuốc" sheetId="10" r:id="rId10"/>
+    <sheet name="In hồ sơ bệnh án" sheetId="11" r:id="rId11"/>
+    <sheet name="Ghi kết quả xét nghiệm" sheetId="12" r:id="rId12"/>
+    <sheet name="In kết quả xét nghiệm" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Đăng nhập'!$A$1:$AA$38</definedName>
@@ -148,6 +156,204 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82D11A94-979D-499C-87A1-3D3CE9EB0855}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3649980" cy="3345180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9CB7963-1AD9-41A9-8345-939CB25BAE8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3931920" cy="6210300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE32525-1050-46B2-84AD-DBE566EDAC91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3535680" cy="3345180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -159,16 +365,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="http://www.plantuml.com/plantuml/png/hL1BJiGm3Dtd5Bu05vW56caM8yG293vxateWmhL7ZalLsvCsKXXGOCMYKUBtUNxTPqVpQUI0qTNWE57s45NSbE7uT1D8FFa2z-YfN7C8PGXNrvMvWuStdI4QeHESrCQmpGjX5U_WSJaJdAiMagoCyb3vGJjmYkzmTmilatj1ox1XpyXfGATBUNS9bLEoiMw1x1M4k5bd_A1gterk-5TuQrpiLr1eRaMCejeGY3DzIuaeaVYNd0wZqs96aoIlhSK_-VV_qaM1GK6qvlpjSc0jeYgNOVlsvPX6_WG0">
+        <xdr:cNvPr id="3" name="Picture 2" descr="PlantUML diagram">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B67C613B-AE7B-4F95-A1F0-099780304417}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A283D35-93AA-4206-8D83-98CE9460BEFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -231,10 +437,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="PlantUML diagram">
+        <xdr:cNvPr id="3" name="Picture 2" descr="PlantUML diagram">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F32A50-4E49-4DCE-A07D-4169B0F0F386}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33F6A11-0CE2-49C9-8717-E429853448BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -390,7 +596,271 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5715000" cy="3497580"/>
+          <a:ext cx="5715000" cy="3401060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4594A3A4-B3C1-4807-8EB2-7C8B56B6CDDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5181600" cy="8001000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D2CD3EE-0C89-41C8-AC05-E9C7D456D85D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2964180" cy="3931920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{305767F8-52EF-43F4-B2D4-7B3D4F2E48F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4259580" cy="3771900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="PlantUML diagram">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB2FB19A-9445-4201-9FA2-634DCA23CE50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5440680" cy="7620000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -711,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F24E4CC-8333-476B-A51C-55FE6CBD97F7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="AJ20" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
@@ -723,12 +1193,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8EAEDF-0EA0-4170-A5F4-F9902CADEE0C}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69384CB2-60A5-491D-8F8F-529C89ED4A60}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A24" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="Z35" sqref="Z35"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47150D6B-8BF2-49D5-9698-2724AE23D979}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E14B361-9E2D-4B2E-9D26-6F2BD2904BAF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM13" sqref="AM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,11 +1237,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8ADAF7-11CC-4E2A-8314-C5C46C83AC81}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94EC592-1129-40B5-993F-E7F98D114EF6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A52" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8EAEDF-0EA0-4170-A5F4-F9902CADEE0C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -753,11 +1264,39 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8ADAF7-11CC-4E2A-8314-C5C46C83AC81}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B270ABBF-CFBE-4B5D-987F-5D1C31AEA171}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C40D82A-8095-48C5-A7A8-2C7DE15E135C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="AQ42" sqref="AQ42"/>
     </sheetView>
   </sheetViews>
@@ -769,17 +1308,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC7C155-04ED-45BC-9349-677541BBB354}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM9" sqref="AM9"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D63739-80BC-4307-9BE7-8DDE568F3539}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4737EC5-8DC5-47DB-AA97-6E0DD7BE2F54}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC24" sqref="AC24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0686781-83C8-4E63-91B5-DA996E50D9CC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>